<commit_message>
nya produkt bilder och uppdaterad excel
pushar upp nya produkt bilder med en ny kategori samt uppdaterad excel
</commit_message>
<xml_diff>
--- a/wp-content/themes/SAD_Active/produktbilder/produkter.xlsx
+++ b/wp-content/themes/SAD_Active/produktbilder/produkter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffdb61f3ca5e596b/Gemensamma dokument/3.8. Skolan/WEBB-E-HANDEL/Repos/wp_mockup_webshop/produktbilder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\Wordpress---Webshop\wp-content\themes\SAD_Active\produktbilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{47A09C1F-6B93-4F97-B075-979B61F829BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DCBE89A-B2C4-4209-A0FC-AADD20C6D7CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85380F7C-F7BA-4350-8EDD-EA6E93E6B5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>Produktnamn</t>
   </si>
@@ -36,39 +36,10 @@
     <t>beskrivning</t>
   </si>
   <si>
-    <t>Cloudfoam Pure 2.0 Cloud</t>
-  </si>
-  <si>
     <t>Dam</t>
   </si>
   <si>
-    <t>Eq21 Run Dash Grey</t>
-  </si>
-  <si>
-    <t>Eq21 Run Dash Grey2</t>
-  </si>
-  <si>
-    <t>Löparskor för ultimat komfort.
-Med de här löparskorna från adidas kan du njuta av skön komfort kilometer efter kilometer. Den ventilerande ovandelen håller fötterna fräscha under långa löprundor. Lätt stötdämpning ger bekväm fjädring i steget från första frånskjutet till sista nedtrampet. Den här produkten är gjord i återvunnet material som en del av vår ambition att sätta stopp för plastavfallet. Tjugo procent av de delar som använts för att tillverka ovandelen är gjorda i minst femtio procent återvunnet material.</t>
-  </si>
-  <si>
-    <t>Puremotion Adapt</t>
-  </si>
-  <si>
-    <t>Racer Tr21 Cloud</t>
-  </si>
-  <si>
     <t>Herr</t>
-  </si>
-  <si>
-    <t>Skor för vardagskomfort.
-Med de här skorna kan du njuta av bekväma och lätta steg hela dagen. Löparinspirerad stötdämpning med låg vikt. Designen med 3-Stripes ger en klassisk adidaslook som passar alla stilar. Den här produkten är gjord med Primegreen, en serie med mycket funktionella, återvunna material. 50 % av ovandelen utgörs av återvunnet material. Ingen nyproducerad polyester.</t>
-  </si>
-  <si>
-    <t>Ultraboost Pb Core Black</t>
-  </si>
-  <si>
-    <t>Här är din nya bästa vän för dina snabbaste och längsta löpturer. Den eleganta silhuetten och den responsiva komforten hos Ultraboost gör dig redo för tävlingar och allt du kan tänka dig. Dessa Ultraboost PB-skor har en ovansida gjord av den lättaste mesh som adidas har. Invärtes stöd låser fast passformen när du spurtar mot mål. 3 ränder inspirerade av japansk kalligrafi bidrar till den snabba känslan.</t>
   </si>
   <si>
     <t>bild1</t>
@@ -115,33 +86,6 @@
   </si>
   <si>
     <t>Own_The_Run_Tight_Pb_3_Stripes_Women_Black2</t>
-  </si>
-  <si>
-    <t>Cloudfoam_Pure_2.0</t>
-  </si>
-  <si>
-    <t>Cloudfoam_Pure_2.02</t>
-  </si>
-  <si>
-    <t>Eq21_Run_Dash_Grey</t>
-  </si>
-  <si>
-    <t>Puremotion_Adapt</t>
-  </si>
-  <si>
-    <t>Puremotion_Adapt2</t>
-  </si>
-  <si>
-    <t>Racer _Tr21_Cloud2</t>
-  </si>
-  <si>
-    <t>Racer _Tr21_Cloud</t>
-  </si>
-  <si>
-    <t>Ultraboost_Pb_Core_Black</t>
-  </si>
-  <si>
-    <t>Ultraboost_Pb_Core_Black2</t>
   </si>
   <si>
     <t>Run It Tight 7-8 3 Stripe Women Black</t>
@@ -255,26 +199,9 @@
 Ficka för nycklar</t>
   </si>
   <si>
-    <t>Sportiga skor med supermjuk Cloudfoam-dämpning.
-De här skorna ger en fräsch, ren stil och komfort. De här löparinspirerade skorna är gjorda i en avslappnad, sval och samlad stil tack vare adidas klassiska vibbar. Oavsett om du hänger med vänner eller försöker att hinna med allt på helgens att-göra-lista, så är du bekväm hela tiden. Den här produkten är gjord med Primegreen, en serie med mycket funktionella, återvunna material.</t>
-  </si>
-  <si>
-    <t>adidasskor med en stretchig ovandel. 
-Stick in fötterna och njut av den sofistikerade designen. De här löparinspirerade skorna kombinerar en praktisk, snörlös stängning med en stilren look. Mjuk stötdämpning ger en bekväm känsla när du behöver vara på språng längre än väntat. Den här produkten är gjord i återvunnet material som en del av vår ambition att sätta stopp för plastavfallet. Tjugo procent av de delar som använts för att tillverka ovandelen är gjorda i minst femtio procent återvunnet material.</t>
-  </si>
-  <si>
-    <t>Skor:</t>
-  </si>
-  <si>
     <t>Underdel:</t>
   </si>
   <si>
-    <t>Överdel:</t>
-  </si>
-  <si>
-    <t>Kolumn1</t>
-  </si>
-  <si>
     <t>top_men_1_black</t>
   </si>
   <si>
@@ -302,22 +229,107 @@
     <t>pants_women_3_black</t>
   </si>
   <si>
-    <t>shoes_women_1</t>
-  </si>
-  <si>
-    <t>shoes_men_1</t>
-  </si>
-  <si>
-    <t>shoes_women_2</t>
-  </si>
-  <si>
-    <t>shoes_women_3</t>
-  </si>
-  <si>
-    <t>shoes_men_2</t>
-  </si>
-  <si>
-    <t>top_women_3_black</t>
+    <t>Tröjor</t>
+  </si>
+  <si>
+    <t>Jackor</t>
+  </si>
+  <si>
+    <t>Marathon_Jacket_Translucent_Women_Black</t>
+  </si>
+  <si>
+    <t>Marathon Jacket Translucent Women Black</t>
+  </si>
+  <si>
+    <t>Terrex_Parley_Agravic_Tr_Wind_Rdy_Windbreaker_Mesa</t>
+  </si>
+  <si>
+    <t>Terrex_Parley_Agravic_Tr_Wind_Rdy_Windbreaker_Mesa2</t>
+  </si>
+  <si>
+    <t>Blocked_Longsleeve_Tee_Women_Wonder_White</t>
+  </si>
+  <si>
+    <t>Blocked_Longsleeve_Tee_Women_Wonder_White2</t>
+  </si>
+  <si>
+    <t>Blocked Longsleeve Tee Women Wonder White</t>
+  </si>
+  <si>
+    <t>Own the Run Tee Black</t>
+  </si>
+  <si>
+    <t>Own_the_Run_Tee_Black</t>
+  </si>
+  <si>
+    <t>Own_the_Run_Tee_Black2</t>
+  </si>
+  <si>
+    <t>Reflective LS Black</t>
+  </si>
+  <si>
+    <t>Reflective_LS_Black</t>
+  </si>
+  <si>
+    <t>Reflective_LS_Black2</t>
+  </si>
+  <si>
+    <t>En löpartröja som är utrustad för svalt väder.
+Din löprunda behöver inte pausa. Lite kyla i luften kan inte stoppa dig. Dra på dig den här löpartröjan från adidas och njut av löpning i kyligt väder. AEROREADY absorberar fukt för att hålla dig torr och den höga kragen värmer skönt. Reflexdetaljer lyser när du tränar i gryningen eller när solen går ner. Den här produkten är gjord med Primegreen, en serie med mycket funktionella, återvunna material.
+Normal passform
+Polokrage
+Jacquard i 100 % återvunnen polyester
+Fuktabsorberande
+Tumhål på muddar</t>
+  </si>
+  <si>
+    <t>Inse din potential i denna lätta löpartröja. Strategiskt placerad ventilation håller dig sval och torr under hela löprundan. Förformade ärmbågar följer kroppens former och tumhål ger extra skydd.</t>
+  </si>
+  <si>
+    <t>En löparjacka med huva för träning i vind och regn.
+Förbered dig för långlöpningar. Även de blöta och blåsiga. Dra på det lätta och ventilerande skyddet i den här löparjackan från adidas, gjord i återvunnet material. Du kommer att känna dig torr och trygg, även om vädret inte är det.
+Normal passform
+Hel dragkedja och huva
+Dubbelväv i 100 % återvunnen polyester med slitstarkt, vattenavvisande DWR-överdrag
+Lätt och ventilerande
+Fickor med dragkedja framtill
+Packbar ficka och svettskyddad mobilficka</t>
+  </si>
+  <si>
+    <t>Terrex Parley Agravic Tr Wind.Rdy Windbreaker Mesa</t>
+  </si>
+  <si>
+    <t>En vindjacka för traillöpning som är enkel att packa med.
+Den här vindjackan för traillöpning från adidas Terrex ger dig ytterligare en anledning att ge dig ut i spåret när vädret är ett argument för att stanna hemma. WIND.RDY står emot vind för en bekväm känsla när det blåser och är fuktigt. Den lätta designen gör att den enkelt kan packas ner i en ficka. Den här produkten är gjord med Parley Ocean Plastic, skapat av återvunnet plastavfall insamlat från avlägsna öar, stränder, kustområden och kustlinjer, för att förhindra att det når haven.
+Normal passform
+Hel dragkedja och ståkrage
+Dubbelväv i 100 % återvunnen polyester med slitstarkt, vattenavvisande DWR-överdrag
+Sidosömsfickor med dragkedja
+Jackan går att vika ihop i sin egen ficka</t>
+  </si>
+  <si>
+    <t>För dig som inte ser löpning som en säsongsaktivitet. Kör året runt och få ditt träningspass att bli av varje dag i denna långärmade adidas löpar-t-shirt. Håll dig bekväm med fukttransporterande tyg. Tumhål i manschetter. Reflekterande detaljer. Polokrage. 100 % återvunnet polyester falsk hålsöm. Långärmad t-shirt för löpning. Fuktabsorberande AEROREADY.</t>
+  </si>
+  <si>
+    <t>jacket_women_3_black</t>
+  </si>
+  <si>
+    <t>jacket_women_1_black</t>
+  </si>
+  <si>
+    <t>jacket_women_2_black</t>
+  </si>
+  <si>
+    <t>jacket_men_2_black</t>
+  </si>
+  <si>
+    <t>jacket_men_1_black</t>
+  </si>
+  <si>
+    <t>top_women_1_white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU </t>
   </si>
 </sst>
 </file>
@@ -346,18 +358,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -372,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -381,11 +387,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,11 +446,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{966C6F42-C86E-4832-8C2A-8125266D49AB}" name="Table1" displayName="Table1" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20" xr:uid="{966C6F42-C86E-4832-8C2A-8125266D49AB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{966C6F42-C86E-4832-8C2A-8125266D49AB}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{966C6F42-C86E-4832-8C2A-8125266D49AB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3F49D0FC-175B-423B-A28F-85012EEC6784}" name="Produktnamn"/>
-    <tableColumn id="2" xr3:uid="{E9C88BD3-CF04-4783-A7E5-09F4471904F0}" name="Kolumn1"/>
+    <tableColumn id="2" xr3:uid="{E9C88BD3-CF04-4783-A7E5-09F4471904F0}" name="SKU "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,7 +487,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -781,7 +786,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,19 +806,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -821,368 +826,372 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>619</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D3">
+        <v>1329</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4">
-        <v>749</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
+      <c r="D4">
+        <v>1059</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>929</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>389</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
-        <v>479</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4">
-        <v>619</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1319</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
+      <c r="D7">
+        <v>589</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>439</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>479</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>439</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4">
-        <v>439</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="G11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>319</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>339</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>479</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>439</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4">
-        <v>319</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4">
-        <v>339</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="G13" s="5" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B14" s="3"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>314</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="4">
-        <v>314</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="D16">
         <v>419</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>48</v>
+      <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4">
-        <v>389</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>254</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>539</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1059</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>1329</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>60</v>
+        <v>374</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>